<commit_message>
Product backlog creation, sprint 2 closing and starting sprint 3
</commit_message>
<xml_diff>
--- a/Documentation/Product Backlog.xlsx
+++ b/Documentation/Product Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nevidjen\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nevidjen\Documents\GitHub\MasterAudioTechnologyFunctions\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>Id</t>
   </si>
@@ -36,6 +36,102 @@
   </si>
   <si>
     <t>Note</t>
+  </si>
+  <si>
+    <t>Implement tracks functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Playing music and flow control </t>
+  </si>
+  <si>
+    <t>Implement basic GUI</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>Logo an basic appereance</t>
+  </si>
+  <si>
+    <t>Documentation template that professor requires</t>
+  </si>
+  <si>
+    <t>Basic audio file playing</t>
+  </si>
+  <si>
+    <t>Basic GUI required for further development</t>
+  </si>
+  <si>
+    <t>Create app marketing design</t>
+  </si>
+  <si>
+    <t>Write documetation for proffesor</t>
+  </si>
+  <si>
+    <t>Implementing tracks for audio mixing (multiple audio playing)</t>
+  </si>
+  <si>
+    <t>Create virtual MIDI keyboard</t>
+  </si>
+  <si>
+    <t>Sprint ready</t>
+  </si>
+  <si>
+    <t>Not sprint ready</t>
+  </si>
+  <si>
+    <t>Create keyboard for playing custom melodies and implement them in track</t>
+  </si>
+  <si>
+    <t>Improve GUI design</t>
+  </si>
+  <si>
+    <t>Redesign buttons and GUI in general</t>
+  </si>
+  <si>
+    <t>Implement project file format</t>
+  </si>
+  <si>
+    <t>Save and open project file custom format (.matf)</t>
+  </si>
+  <si>
+    <t>Add support for other sound file formats</t>
+  </si>
+  <si>
+    <t>Implement final GUI design</t>
+  </si>
+  <si>
+    <t>For mp3, ogg, ac3, aiff, wma etc</t>
+  </si>
+  <si>
+    <t>Custom, designed, implementation of GUI</t>
+  </si>
+  <si>
+    <t>Design buttons faces for GUI</t>
+  </si>
+  <si>
+    <t>Redesgn buttons in png format</t>
+  </si>
+  <si>
+    <t>Exporting project to popular audio formats</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Exporting mixed audio file</t>
   </si>
 </sst>
 </file>
@@ -158,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -173,24 +269,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="4">
     <dxf>
       <font>
-        <color theme="7" tint="-0.24994659260841701"/>
+        <color theme="8" tint="-0.499984740745262"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <color theme="9" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="8" tint="-0.499984740745262"/>
       </font>
     </dxf>
     <dxf>
@@ -205,22 +305,7 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
+        <color theme="7" tint="-0.24994659260841701"/>
       </font>
     </dxf>
   </dxfs>
@@ -533,20 +618,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="43.5703125" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="67.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -554,182 +640,301 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <f>A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <f t="shared" ref="A5:A18" si="0">A4+1</f>
         <v>4</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" s="5"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="5"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"Not sprint ready"</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"Sprint ready"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
-      <formula>"Not sprint ready"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"In progress"</formula>
-    </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
       <formula1>"Sprint ready, Not sprint ready,Completed,In progress,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C18">
+      <formula1>"High,Medium,Low,"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>